<commit_message>
Update the master info
</commit_message>
<xml_diff>
--- a/dt_surveys_master/survey_mastersheet_info.xlsx
+++ b/dt_surveys_master/survey_mastersheet_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aflub\Desktop\prj_LSHTM_study\prj_sc_model_comparison\dt_surveys_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D0482-065C-42AE-B313-A47D2D1DF1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3996C2A-50AA-4D0F-82FB-505C2B4D9739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="390" windowWidth="24570" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8145" yWindow="540" windowWidth="20250" windowHeight="15015" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="482">
   <si>
     <t>title</t>
     <phoneticPr fontId="2"/>
@@ -2737,6 +2737,182 @@
   </si>
   <si>
     <t>Danon_2013_online</t>
+  </si>
+  <si>
+    <t>Country or region</t>
+  </si>
+  <si>
+    <t>Data collection period</t>
+  </si>
+  <si>
+    <t>May 2005 - September 2006</t>
+  </si>
+  <si>
+    <t>Eight UK and European countries</t>
+  </si>
+  <si>
+    <t>Country or region, raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">different commercial companies or public health institutes in Belgium (BE), Germany
+(DE), Finland (FI), Great Britain (GB), Italy (IT), Luxembourg
+(LU), The Netherlands (NL), and Poland (PL). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The surveys were conducted between May
+2005 and September 2006</t>
+  </si>
+  <si>
+    <t>Data collection period, raw</t>
+  </si>
+  <si>
+    <t>Over the period March – May 2006, 750 persons living in
+Belgium were recruited by random digit dialing on fixed
+telephone lines.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See cnt, reg. </t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0118457</t>
+  </si>
+  <si>
+    <t>Zotero install</t>
+  </si>
+  <si>
+    <t>the province of San Marcos, Department of Cajamarca, in the
+northern highlands of Peru.</t>
+  </si>
+  <si>
+    <t>Eligibility</t>
+  </si>
+  <si>
+    <t>San Marcos’ households with children younger than 3 years of age (index children)</t>
+  </si>
+  <si>
+    <t>were enrolled and followed
+through weekly household visits from May 2009 through September 2011.</t>
+  </si>
+  <si>
+    <t>May 2009 - September 2011</t>
+  </si>
+  <si>
+    <t>The study was conducted as part of the sixth round of the Manicaland HIV/STD Prevention
+Study [36], a general population cohort study carried out between 1998 and 2013 in Manicaland, the easternmost province of Zimbabwe.</t>
+  </si>
+  <si>
+    <t>Data were gathered from March 2013 to August 2013</t>
+  </si>
+  <si>
+    <t>March 2013 to August 2013</t>
+  </si>
+  <si>
+    <t>general population cohort study carried out between 1998 and 2013 in Manicaland, the easternmost province of Zimbabwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> randomly sampled from all over France</t>
+  </si>
+  <si>
+    <t>planned over 2 time periods (February-March/April-May 2012) (Fig 1). An oversight
+leading to recruit fewer participants than originally planned during the February-March period
+(Actual Period 1), an additional period (Actual Period 2) was added in April to complete“Design Period 1”. Recruitment during “Design Period 2” was completed according to plan
+(Actual Period 3).</t>
+  </si>
+  <si>
+    <t>March - May 2012</t>
+  </si>
+  <si>
+    <t>We conducted a population-based
+social contact survey in Hong Kong</t>
+  </si>
+  <si>
+    <t>population-based social contact survey in 2015/16</t>
+  </si>
+  <si>
+    <t>In 2007 a household-based cohort was established in a semirural community in the Red River Delta of North Vietnam.</t>
+  </si>
+  <si>
+    <t>final tuberculosis prevalence survey that was carried out in
+2010 in 16 communities in Zambia and 8 communities in
+the Western Cape, South Africa, were randomly selected for
+face-to-face interviews.</t>
+  </si>
+  <si>
+    <t>The survey was carried out between December 2017 and May 2018 in Shanghai, a city in the
+southeast of China</t>
+  </si>
+  <si>
+    <t>San Marcos, Peru</t>
+  </si>
+  <si>
+    <t>Manicaland, Zimbabwe</t>
+  </si>
+  <si>
+    <t>Zambia and Western Cap, South Africa</t>
+  </si>
+  <si>
+    <t>Shanghai, China</t>
+  </si>
+  <si>
+    <t>Social contact data were obtained in Flanders between
+September 2010 and February 2011 and covered two school
+holiday periods.</t>
+  </si>
+  <si>
+    <t>Flanders, Belgium</t>
+  </si>
+  <si>
+    <t>The survey was conducted in various workplaces in Pathum Thani, Thailand, between September
+and November 2015.</t>
+  </si>
+  <si>
+    <t>The target population was migrant workers from Cambodia, Lao People’s
+Democratic Republic (Lao PDR), and Myanmar who were willing to participate and signed informed
+consent forms.</t>
+  </si>
+  <si>
+    <t>https://projecteuclid.org/journals/annals-of-applied-statistics/volume-11/issue-1/Efficient-estimation-of-age-specific-social-contact-rates-between-men/10.1214/16-AOAS1006.full</t>
+  </si>
+  <si>
+    <t>Data were collected within the POLYMOD
+multi-country study. only 269 of
+these 825 Dutch participants were included in the study published</t>
+  </si>
+  <si>
+    <t>Data collection took place in 2006 and 2007.</t>
+  </si>
+  <si>
+    <t>We conducted a cross-sectional survey of households and individuals within GB</t>
+  </si>
+  <si>
+    <t>Great Briain, United Kingdom</t>
+  </si>
+  <si>
+    <t>with a total of 140 000 posted during 2009</t>
+  </si>
+  <si>
+    <t>Participants were recruited from randomly selected households, in
+40 communities in a transect spanning a gradient of decreasing
+population density extending to the northeast of Guangzhou,
+China.</t>
+  </si>
+  <si>
+    <t>Guangdong, China</t>
+  </si>
+  <si>
+    <t>During 2009 and 2010, we conducted a study
+of human contact patterns in a spatially random sample of communities in and around Guangzhou, China</t>
+  </si>
+  <si>
+    <t>2009 - 2010</t>
+  </si>
+  <si>
+    <t>Willem_2012</t>
+  </si>
+  <si>
+    <t>https://www.ecdc.europa.eu/en/publications-data/social-contact-patterns-eueea-during-covid-19-pandemic</t>
   </si>
 </sst>
 </file>
@@ -3197,11 +3373,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5792,13 +5968,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F91536-BFB3-45D6-A52E-7141CA7681FC}">
-  <dimension ref="A1:AF28"/>
+  <dimension ref="A1:AL28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="S14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -5806,19 +5982,19 @@
     <col min="1" max="1" width="9.140625" style="9"/>
     <col min="2" max="2" width="16.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="12"/>
-    <col min="4" max="4" width="17" style="12" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="12" customWidth="1"/>
-    <col min="6" max="8" width="19.85546875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="34.140625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="41.85546875" style="12" customWidth="1"/>
-    <col min="11" max="11" width="41.140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="50.7109375" style="12" customWidth="1"/>
-    <col min="13" max="14" width="17" style="12" customWidth="1"/>
-    <col min="15" max="16" width="17" style="9" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="9" width="17" style="12" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" style="12" customWidth="1"/>
+    <col min="11" max="13" width="19.85546875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="34.140625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="41.85546875" style="12" customWidth="1"/>
+    <col min="16" max="16" width="41.140625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="50.7109375" style="12" customWidth="1"/>
+    <col min="18" max="19" width="17" style="12" customWidth="1"/>
+    <col min="20" max="22" width="17" style="9" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="24">
+    <row r="1" spans="1:38" ht="24">
       <c r="A1" s="5" t="s">
         <v>58</v>
       </c>
@@ -5832,50 +6008,62 @@
         <v>0</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="V1" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="W1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
@@ -5885,8 +6073,14 @@
       <c r="AD1" s="8"/>
       <c r="AE1" s="8"/>
       <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
     </row>
-    <row r="2" spans="1:32" ht="132">
+    <row r="2" spans="1:38" ht="180">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5899,51 +6093,61 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="O2" s="5">
+      <c r="T2" s="5">
         <v>7290</v>
       </c>
-      <c r="P2" s="5">
+      <c r="U2" s="5">
         <v>7254</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="V2" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W2" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
@@ -5953,8 +6157,14 @@
       <c r="AD2" s="8"/>
       <c r="AE2" s="8"/>
       <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
     </row>
-    <row r="3" spans="1:32" ht="204">
+    <row r="3" spans="1:38" ht="204">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -5968,50 +6178,60 @@
         <v>7</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="O3" s="5">
+      <c r="T3" s="5">
         <v>750</v>
       </c>
-      <c r="P3" s="5">
+      <c r="U3" s="5">
         <v>1496</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="V3" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
@@ -6021,8 +6241,14 @@
       <c r="AD3" s="8"/>
       <c r="AE3" s="8"/>
       <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
     </row>
-    <row r="4" spans="1:32" ht="120">
+    <row r="4" spans="1:38" ht="120">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -6036,50 +6262,62 @@
         <v>10</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="O4" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="O4" s="5">
+      <c r="T4" s="5">
         <v>588</v>
       </c>
-      <c r="P4" s="5">
+      <c r="U4" s="5">
         <v>568</v>
       </c>
-      <c r="Q4" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
+      <c r="V4" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>443</v>
+      </c>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
@@ -6089,8 +6327,14 @@
       <c r="AD4" s="8"/>
       <c r="AE4" s="8"/>
       <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
     </row>
-    <row r="5" spans="1:32" ht="156">
+    <row r="5" spans="1:38" ht="156">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -6103,51 +6347,63 @@
       <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="R5" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="O5" s="5">
+      <c r="T5" s="5">
         <v>1245</v>
       </c>
-      <c r="P5" s="5">
+      <c r="U5" s="5">
         <v>1241</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="V5" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
@@ -6157,8 +6413,14 @@
       <c r="AD5" s="8"/>
       <c r="AE5" s="8"/>
       <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
     </row>
-    <row r="6" spans="1:32" ht="168">
+    <row r="6" spans="1:38" ht="264">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -6172,50 +6434,60 @@
         <v>17</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="O6" s="5">
+      <c r="T6" s="5">
         <v>1755</v>
       </c>
-      <c r="P6" s="5">
+      <c r="U6" s="5">
         <v>3464</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="V6" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W6" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
@@ -6225,8 +6497,14 @@
       <c r="AD6" s="8"/>
       <c r="AE6" s="8"/>
       <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
     </row>
-    <row r="7" spans="1:32" ht="120">
+    <row r="7" spans="1:38" ht="120">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6240,50 +6518,60 @@
         <v>21</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="M7" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="O7" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="R7" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="S7" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="O7" s="5">
+      <c r="T7" s="5">
         <v>1149</v>
       </c>
-      <c r="P7" s="5">
+      <c r="U7" s="5">
         <v>1149</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="V7" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W7" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
@@ -6293,8 +6581,14 @@
       <c r="AD7" s="8"/>
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
     </row>
-    <row r="8" spans="1:32" ht="120">
+    <row r="8" spans="1:38" ht="120">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6308,50 +6602,60 @@
         <v>25</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2007</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="M8" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="N8" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="R8" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="N8" s="11">
+      <c r="S8" s="11">
         <v>2007</v>
       </c>
-      <c r="O8" s="5">
+      <c r="T8" s="5">
         <v>865</v>
       </c>
-      <c r="P8" s="5">
+      <c r="U8" s="5">
         <v>865</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="V8" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W8" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
@@ -6361,8 +6665,14 @@
       <c r="AD8" s="8"/>
       <c r="AE8" s="8"/>
       <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
     </row>
-    <row r="9" spans="1:32" ht="36">
+    <row r="9" spans="1:38" ht="36">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -6375,37 +6685,37 @@
       <c r="D9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="S9" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="O9" s="5">
+      <c r="T9" s="5">
         <v>116</v>
       </c>
-      <c r="P9" s="5">
+      <c r="U9" s="5">
         <v>116</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="V9" s="6"/>
+      <c r="W9" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
@@ -6415,8 +6725,14 @@
       <c r="AD9" s="8"/>
       <c r="AE9" s="8"/>
       <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
     </row>
-    <row r="10" spans="1:32" ht="144">
+    <row r="10" spans="1:38" ht="168">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -6430,50 +6746,60 @@
         <v>33</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H10" s="11">
+        <v>2010</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="K10" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="L10" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="M10" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="N10" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="O10" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="P10" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="Q10" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="R10" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="S10" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="O10" s="5">
+      <c r="T10" s="5">
         <v>3576</v>
       </c>
-      <c r="P10" s="5">
+      <c r="U10" s="5">
         <v>3470</v>
       </c>
-      <c r="Q10" s="18" t="s">
+      <c r="V10" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W10" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
@@ -6483,8 +6809,14 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
     </row>
-    <row r="11" spans="1:32" ht="144">
+    <row r="11" spans="1:38" ht="144">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -6498,50 +6830,60 @@
         <v>36</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="M11" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="N11" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="O11" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="P11" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="Q11" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="R11" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="S11" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="O11" s="5">
+      <c r="T11" s="5">
         <v>965</v>
       </c>
-      <c r="P11" s="5">
+      <c r="U11" s="5">
         <v>955</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="V11" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W11" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
@@ -6551,8 +6893,14 @@
       <c r="AD11" s="8"/>
       <c r="AE11" s="8"/>
       <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
     </row>
-    <row r="12" spans="1:32" ht="132">
+    <row r="12" spans="1:38" ht="144">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -6565,37 +6913,39 @@
       <c r="D12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="S12" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="O12" s="5">
+      <c r="T12" s="5">
         <v>631</v>
       </c>
-      <c r="P12" s="5">
+      <c r="U12" s="5">
         <v>631</v>
       </c>
-      <c r="Q12" s="10" t="s">
+      <c r="V12" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W12" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
       <c r="X12" s="8"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
@@ -6605,13 +6955,19 @@
       <c r="AD12" s="8"/>
       <c r="AE12" s="8"/>
       <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
     </row>
-    <row r="13" spans="1:32" ht="84">
+    <row r="13" spans="1:38" ht="84">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>144</v>
+        <v>480</v>
       </c>
       <c r="C13" s="11">
         <v>2012</v>
@@ -6620,50 +6976,60 @@
         <v>43</v>
       </c>
       <c r="E13" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="L13" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="M13" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="N13" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="O13" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="P13" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="Q13" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="R13" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="S13" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="O13" s="5">
+      <c r="T13" s="5">
         <v>1759</v>
       </c>
-      <c r="P13" s="5">
+      <c r="U13" s="5">
         <v>1744</v>
       </c>
-      <c r="Q13" s="18" t="s">
+      <c r="V13" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W13" s="18" t="s">
         <v>379</v>
       </c>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
       <c r="X13" s="8"/>
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
@@ -6673,8 +7039,14 @@
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
       <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="8"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
     </row>
-    <row r="14" spans="1:32" ht="156">
+    <row r="14" spans="1:38" ht="156">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6688,50 +7060,62 @@
         <v>46</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="L14" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="M14" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="N14" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="O14" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="P14" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="Q14" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="R14" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="S14" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="O14" s="5">
+      <c r="T14" s="5">
         <v>369</v>
       </c>
-      <c r="P14" s="5">
+      <c r="U14" s="5">
         <v>369</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="V14" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W14" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
@@ -6741,8 +7125,14 @@
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
       <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
     </row>
-    <row r="15" spans="1:32" ht="144">
+    <row r="15" spans="1:38" ht="144">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -6755,51 +7145,61 @@
       <c r="D15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="K15" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="L15" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="M15" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="N15" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="O15" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="P15" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="Q15" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="R15" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="S15" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="O15" s="5">
+      <c r="T15" s="5">
         <v>825</v>
       </c>
-      <c r="P15" s="5">
+      <c r="U15" s="5">
         <v>821</v>
       </c>
-      <c r="Q15" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
+      <c r="V15" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W15" s="18" t="s">
+        <v>470</v>
+      </c>
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
@@ -6809,8 +7209,14 @@
       <c r="AD15" s="8"/>
       <c r="AE15" s="8"/>
       <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="8"/>
+      <c r="AI15" s="8"/>
+      <c r="AJ15" s="8"/>
+      <c r="AK15" s="8"/>
+      <c r="AL15" s="8"/>
     </row>
-    <row r="16" spans="1:32" ht="24">
+    <row r="16" spans="1:38" ht="24">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -6831,27 +7237,27 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="O16" s="5">
+      <c r="T16" s="5">
         <v>55923</v>
       </c>
-      <c r="P16" s="5">
+      <c r="U16" s="5">
         <v>227794</v>
       </c>
-      <c r="Q16" s="9" t="s">
+      <c r="V16" s="6"/>
+      <c r="W16" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
@@ -6861,8 +7267,14 @@
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
       <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
+      <c r="AL16" s="8"/>
     </row>
-    <row r="17" spans="1:32" ht="24">
+    <row r="17" spans="1:38" ht="24">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -6885,21 +7297,21 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
-      <c r="O17" s="5">
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="5">
         <v>3996</v>
       </c>
-      <c r="P17" s="5">
+      <c r="U17" s="5">
         <v>3946</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="V17" s="6"/>
+      <c r="W17" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
@@ -6909,8 +7321,14 @@
       <c r="AD17" s="8"/>
       <c r="AE17" s="8"/>
       <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
     </row>
-    <row r="18" spans="1:32" ht="24">
+    <row r="18" spans="1:38" ht="24">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -6933,21 +7351,21 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="5">
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="5">
         <v>22857</v>
       </c>
-      <c r="P18" s="5">
+      <c r="U18" s="5">
         <v>22857</v>
       </c>
-      <c r="Q18" s="10" t="s">
+      <c r="V18" s="6"/>
+      <c r="W18" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
@@ -6957,8 +7375,14 @@
       <c r="AD18" s="8"/>
       <c r="AE18" s="8"/>
       <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="8"/>
+      <c r="AL18" s="8"/>
     </row>
-    <row r="19" spans="1:32" ht="24">
+    <row r="19" spans="1:38" ht="24">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6981,18 +7405,18 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="5">
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="5">
         <v>6319</v>
       </c>
-      <c r="P19" s="5">
+      <c r="U19" s="5">
         <v>6319</v>
       </c>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
+      <c r="V19" s="6"/>
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
@@ -7002,8 +7426,14 @@
       <c r="AD19" s="8"/>
       <c r="AE19" s="8"/>
       <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
+      <c r="AI19" s="8"/>
+      <c r="AJ19" s="8"/>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
     </row>
-    <row r="20" spans="1:32" ht="24">
+    <row r="20" spans="1:38" ht="24">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -7024,18 +7454,18 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="6"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
@@ -7045,8 +7475,14 @@
       <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
       <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
     </row>
-    <row r="21" spans="1:32" ht="24">
+    <row r="21" spans="1:38" ht="24">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -7064,24 +7500,24 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="N21" s="11" t="s">
+      <c r="S21" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5">
+      <c r="T21" s="5"/>
+      <c r="U21" s="5">
         <v>63672</v>
       </c>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
+      <c r="V21" s="6"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
@@ -7091,8 +7527,14 @@
       <c r="AD21" s="8"/>
       <c r="AE21" s="8"/>
       <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:38" ht="15">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -7113,24 +7555,27 @@
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="N22" s="11" t="s">
+      <c r="S22" s="11">
+        <v>2022</v>
+      </c>
+      <c r="T22" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="U22" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="P22" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="3" t="s">
+        <v>481</v>
+      </c>
       <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
@@ -7140,8 +7585,14 @@
       <c r="AD22" s="8"/>
       <c r="AE22" s="8"/>
       <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
     </row>
-    <row r="23" spans="1:32" ht="108">
+    <row r="23" spans="1:38" ht="108">
       <c r="A23" s="20">
         <v>22</v>
       </c>
@@ -7155,50 +7606,60 @@
         <v>258</v>
       </c>
       <c r="E23" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>475</v>
+      </c>
+      <c r="H23" s="21">
+        <v>2009</v>
+      </c>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="K23" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="L23" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="M23" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="I23" s="21" t="s">
+      <c r="N23" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="J23" s="21" t="s">
+      <c r="O23" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="K23" s="21" t="s">
+      <c r="P23" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="L23" s="21" t="s">
+      <c r="Q23" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="M23" s="21" t="s">
+      <c r="R23" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="N23" s="21" t="s">
+      <c r="S23" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="O23" s="20" t="s">
+      <c r="T23" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="P23" s="20" t="s">
+      <c r="U23" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="Q23" s="7" t="s">
+      <c r="V23" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W23" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
@@ -7208,8 +7669,14 @@
       <c r="AD23" s="8"/>
       <c r="AE23" s="8"/>
       <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
     </row>
-    <row r="24" spans="1:32" ht="132.75">
+    <row r="24" spans="1:38" ht="156.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -7219,40 +7686,56 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
+        <v>476</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="K24" s="22" t="s">
         <v>422</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="L24" s="22" t="s">
         <v>351</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="M24" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="N24" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="J24" s="22" t="s">
+      <c r="O24" s="22" t="s">
         <v>425</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="P24" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="Q24" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="R24" s="22" t="s">
         <v>421</v>
       </c>
-      <c r="N24" s="22"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="23" t="s">
+      <c r="S24" s="22"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="W24" s="23" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:38">
       <c r="A25" s="8"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
@@ -7267,11 +7750,17 @@
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:38">
       <c r="A26" s="8"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -7286,11 +7775,17 @@
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:38">
       <c r="A27" s="8"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -7305,11 +7800,17 @@
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:38">
       <c r="A28" s="8"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -7324,32 +7825,39 @@
       <c r="L28" s="22"/>
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{1AB71490-C2A0-4D91-B763-4A6BC7C37AC6}"/>
-    <hyperlink ref="Q5" r:id="rId2" xr:uid="{6159E3E2-8A92-479F-8F23-584ACD63C1BC}"/>
-    <hyperlink ref="Q3" r:id="rId3" xr:uid="{9263062D-FE6D-48AF-AB30-5708193D33E2}"/>
-    <hyperlink ref="Q14" r:id="rId4" xr:uid="{20996B79-3A34-4396-95D6-D7360C68D23F}"/>
-    <hyperlink ref="Q15" r:id="rId5" xr:uid="{E456FEA3-741C-4F79-9EF7-CD080AB46DAB}"/>
-    <hyperlink ref="Q17" r:id="rId6" xr:uid="{9B048C85-2412-4CA7-91E9-7C5B513C0D91}"/>
-    <hyperlink ref="Q9" r:id="rId7" xr:uid="{D71AAD91-E536-4489-863B-45177F86D8E5}"/>
-    <hyperlink ref="Q10" r:id="rId8" xr:uid="{32CE5B04-73A7-49A6-9256-289DEC3EE089}"/>
-    <hyperlink ref="Q11" r:id="rId9" xr:uid="{4523FBF4-FD94-48BA-BE0A-62B1951C6D46}"/>
-    <hyperlink ref="Q12" r:id="rId10" xr:uid="{EC31B0A5-44B9-4BEA-BAE4-943D0FA97174}"/>
-    <hyperlink ref="Q13" r:id="rId11" location="s4" xr:uid="{F1584008-7CF5-4093-BD43-38BB9F3A2038}"/>
-    <hyperlink ref="Q6" r:id="rId12" xr:uid="{EE667D75-7959-4597-B7C6-2CAAF951C0FD}"/>
-    <hyperlink ref="Q7" r:id="rId13" xr:uid="{58684F11-DBFF-4E5D-A540-F792288A2EEE}"/>
-    <hyperlink ref="Q8" r:id="rId14" xr:uid="{E423DFB7-36A5-4436-859F-DBC2A1C1E07A}"/>
-    <hyperlink ref="Q4" r:id="rId15" xr:uid="{E83A9676-5BD0-416B-B57E-12A36933ADC8}"/>
-    <hyperlink ref="Q18" r:id="rId16" location="citeas" xr:uid="{4D02397F-AEF9-40FA-9560-F7DF2959EBE4}"/>
-    <hyperlink ref="Q23" r:id="rId17" location="d195695e1" xr:uid="{4EB8EB89-C904-486D-A73D-0009D0B8C77A}"/>
-    <hyperlink ref="Q24" r:id="rId18" xr:uid="{962EB989-EEBB-4E86-BFBB-80827F313AA8}"/>
+    <hyperlink ref="W2" r:id="rId1" xr:uid="{1AB71490-C2A0-4D91-B763-4A6BC7C37AC6}"/>
+    <hyperlink ref="W5" r:id="rId2" xr:uid="{6159E3E2-8A92-479F-8F23-584ACD63C1BC}"/>
+    <hyperlink ref="W3" r:id="rId3" xr:uid="{9263062D-FE6D-48AF-AB30-5708193D33E2}"/>
+    <hyperlink ref="W14" r:id="rId4" xr:uid="{20996B79-3A34-4396-95D6-D7360C68D23F}"/>
+    <hyperlink ref="W15" r:id="rId5" xr:uid="{E456FEA3-741C-4F79-9EF7-CD080AB46DAB}"/>
+    <hyperlink ref="W17" r:id="rId6" xr:uid="{9B048C85-2412-4CA7-91E9-7C5B513C0D91}"/>
+    <hyperlink ref="W9" r:id="rId7" xr:uid="{D71AAD91-E536-4489-863B-45177F86D8E5}"/>
+    <hyperlink ref="W10" r:id="rId8" xr:uid="{32CE5B04-73A7-49A6-9256-289DEC3EE089}"/>
+    <hyperlink ref="W11" r:id="rId9" xr:uid="{4523FBF4-FD94-48BA-BE0A-62B1951C6D46}"/>
+    <hyperlink ref="W12" r:id="rId10" xr:uid="{EC31B0A5-44B9-4BEA-BAE4-943D0FA97174}"/>
+    <hyperlink ref="W13" r:id="rId11" location="s4" xr:uid="{F1584008-7CF5-4093-BD43-38BB9F3A2038}"/>
+    <hyperlink ref="W6" r:id="rId12" xr:uid="{EE667D75-7959-4597-B7C6-2CAAF951C0FD}"/>
+    <hyperlink ref="W7" r:id="rId13" xr:uid="{58684F11-DBFF-4E5D-A540-F792288A2EEE}"/>
+    <hyperlink ref="W8" r:id="rId14" xr:uid="{E423DFB7-36A5-4436-859F-DBC2A1C1E07A}"/>
+    <hyperlink ref="W4" r:id="rId15" xr:uid="{E83A9676-5BD0-416B-B57E-12A36933ADC8}"/>
+    <hyperlink ref="W18" r:id="rId16" location="citeas" xr:uid="{4D02397F-AEF9-40FA-9560-F7DF2959EBE4}"/>
+    <hyperlink ref="W23" r:id="rId17" location="d195695e1" xr:uid="{4EB8EB89-C904-486D-A73D-0009D0B8C77A}"/>
+    <hyperlink ref="W24" r:id="rId18" xr:uid="{962EB989-EEBB-4E86-BFBB-80827F313AA8}"/>
+    <hyperlink ref="W22" r:id="rId19" xr:uid="{C8D5B5CA-BF37-468C-B601-799DEA8E986E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>